<commit_message>
Update checklist download and documentation
</commit_message>
<xml_diff>
--- a/app/root/static/resources/validator/HICF_checklist/example_manifest.xlsx
+++ b/app/root/static/resources/validator/HICF_checklist/example_manifest.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28120" windowHeight="20160" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28120" windowHeight="20160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Manifest" sheetId="1" r:id="rId1"/>
+    <sheet name="example_manifest_with_unknowns." sheetId="1" r:id="rId1"/>
     <sheet name="Notes" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
   <si>
     <t>isolate</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Accession for the sample</t>
   </si>
   <si>
     <t>Accession for raw data i.e. fastq/bam files</t>
@@ -140,9 +137,6 @@
     <t>other classification</t>
   </si>
   <si>
-    <t>Example description</t>
-  </si>
-  <si>
     <t>Staphylococcus aureus 04-02981</t>
   </si>
   <si>
@@ -202,6 +196,48 @@
   </si>
   <si>
     <t>Describes the health care situation of a human host when the sample was obtained. Must be one of "inpatient" or "community". For non-human host, use "community".</t>
+  </si>
+  <si>
+    <t>ERS000001</t>
+  </si>
+  <si>
+    <t>not available: not collected</t>
+  </si>
+  <si>
+    <t>ERS000002</t>
+  </si>
+  <si>
+    <t>tetracyclin;S;40,erythromycin;R;ge50</t>
+  </si>
+  <si>
+    <t>ERS000003</t>
+  </si>
+  <si>
+    <t>Fully complete metadata</t>
+  </si>
+  <si>
+    <t>Partial metadata</t>
+  </si>
+  <si>
+    <t>Minimal metadata</t>
+  </si>
+  <si>
+    <t>uncultured bacterium</t>
+  </si>
+  <si>
+    <t>carriage</t>
+  </si>
+  <si>
+    <t>community</t>
+  </si>
+  <si>
+    <t>Accepts unknown</t>
+  </si>
+  <si>
+    <t>Accession for the sample, e.g. ERS000001</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
   <si>
     <t>antimicrobial resistance</t>
@@ -297,8 +333,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -377,7 +417,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -407,6 +447,8 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -436,6 +478,8 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -460,8 +504,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -471,7 +515,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="368300" y="6108700"/>
-          <a:ext cx="10452100" cy="7543800"/>
+          <a:ext cx="10452100" cy="10274300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -506,17 +550,16 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng" baseline="0"/>
             <a:t>Notes</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0" u="none"/>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="sng" baseline="0"/>
+            <a:rPr lang="en-US" sz="1100" b="0" u="sng" baseline="0"/>
             <a:t>Mandatory/optional</a:t>
           </a:r>
         </a:p>
@@ -526,19 +569,91 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t>Fields highlighted in </a:t>
+            <a:t>Fields highlighted in green are mandatory. Other fields are optional, subject to the dependencies specified below.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>green</a:t>
+            <a:rPr lang="en-US" sz="1100" b="0" u="sng" baseline="0"/>
+            <a:t>"Accepts unknown"</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t> are mandatory. Other fields are optional, subject to the dependencies specified below.</a:t>
+            <a:t>For some samples, such as historical samples of unknown provenance, it may be impossible to complete all mandatory fields. In such cases the value may be given as one of:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>"not available: not collected": not given because no value was collected</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>"not available: restricted access": not given because the data are restricted</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>"not available: to be reported later": not given but a value will be given at a later stage</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>"not applicable": not given because the checklist does not cover this eventuality</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>"obscured": deliberately not given</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>"temporarily obscured": not given but a value will be given at a later stage</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>These terms are accepted in any of the fields flagged as "Accepts unknown". The taxonomy and scientific name fields do not accept "unknown", but there are terms in the NCBI taxonomy tree to denote unknown species, e.g. ID 77133 represents "uncultured bacterium". Unknown organisms should be represented using similar valid terms from the taxonomy tree.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -580,15 +695,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t>If a sample is flagged as </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" u="none" baseline="0"/>
-            <a:t>not </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t>host associated, the four following fields are not required but "isolation source" becomes mandatory.</a:t>
+            <a:t>If a sample is flagged as not host associated, the four following fields are not required but "isolation source" becomes mandatory.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -606,7 +713,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t>When specifying the antimicrobial resistance for a sample, the field should contain a list of comma-separated values. Each value must contain three semi-colon separated fields: the name of the antibiotic, chosen from a curated list; susceptibility flag, either S (susceptible), I (intermediate), or R (resistant); the minimum inhibitory concentration (MIC) in microgrammes per millilitre (µg/ml). Optionally, a fourth, final field may be added, giving the name or location of the diagnostic centre that performed the resistance analysis.</a:t>
+            <a:t>When specifying the antimicrobial resistance for a sample, the field should contain a list of comma-separated values. Each value must contain three semi-colon separated fields: the name of the antibiotic, chosen from a curated list; susceptibility flag, either S (susceptible), I (intermediate), or R (resistant); the minimum inhibitory concentration (MIC) in microgrammes per millilitre (µg/ml). Optionally, a fourth, final field may be added, giving the name or location of the diagnostic centre that performed the resistance analysis. If the MIC value specifies a limit (e.g. &lt;=2), rather than an absolute value, it may be prefixed by one of: le (&lt;=), lt (&lt;), eq (=), gt (&gt;), ge (&gt;=).</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -615,7 +722,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t>Example: amoxicillin;S;2,piperacillin;S;4;WTSI;tetracycline;R;16;China</a:t>
+            <a:t>Example: amoxicillin;S;2,piperacillin;S;4;WTSI;tetracycline;R;16;China,vancomycin;R;ge32</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -742,6 +849,41 @@
             <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
             <a:t>BRENDA Tissue Ontology (BTO) in the EBI Ontology Browser: http://www.ebi.ac.uk/ontology-lookup/browse.do?ontName=BTO</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>EnvO</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>Environment Ontology: http://environmentontology.org/</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>EnvO in the EBI Ontology Browser: http://www.ebi.ac.uk/ontology-lookup/browse.do?ontName=ENVO</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
@@ -1075,9 +1217,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1133"/>
+  <dimension ref="A1:Z1132"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1117,7 +1259,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>10</v>
@@ -1126,40 +1268,40 @@
         <v>11</v>
       </c>
       <c r="G1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="O1" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S1" s="5" t="s">
         <v>1</v>
@@ -1180,51 +1322,51 @@
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="13">
-        <v>1</v>
+      <c r="B2" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E2" s="4">
         <v>703339</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H2" s="4">
         <v>123</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="O2" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="P2" s="4"/>
       <c r="Q2" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R2" s="4"/>
       <c r="S2" s="4">
@@ -1232,7 +1374,7 @@
       </c>
       <c r="T2" s="4"/>
       <c r="U2" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
@@ -1241,24 +1383,63 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="5"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="4">
+        <v>703339</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
+      <c r="H3" s="4">
+        <v>123</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
+      <c r="Q3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="S3" s="4">
+        <v>630</v>
+      </c>
       <c r="T3" s="4"/>
+      <c r="U3" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
@@ -1266,21 +1447,54 @@
       <c r="Z3" s="4"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="C4" s="2"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="4">
+        <v>77133</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
+      <c r="I4" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
+      <c r="Q4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
       <c r="V4" s="4"/>
@@ -1482,6 +1696,8 @@
       <c r="Z12" s="4"/>
     </row>
     <row r="13" spans="1:26">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="2"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -30599,32 +30815,6 @@
       <c r="Y1132" s="4"/>
       <c r="Z1132" s="4"/>
     </row>
-    <row r="1133" spans="1:26">
-      <c r="A1133" s="4"/>
-      <c r="B1133" s="4"/>
-      <c r="C1133" s="2"/>
-      <c r="D1133" s="4"/>
-      <c r="E1133" s="4"/>
-      <c r="F1133" s="4"/>
-      <c r="G1133" s="4"/>
-      <c r="H1133" s="4"/>
-      <c r="J1133" s="4"/>
-      <c r="K1133" s="4"/>
-      <c r="L1133" s="4"/>
-      <c r="M1133" s="4"/>
-      <c r="N1133" s="4"/>
-      <c r="O1133" s="4"/>
-      <c r="P1133" s="4"/>
-      <c r="Q1133" s="4"/>
-      <c r="R1133" s="4"/>
-      <c r="S1133" s="4"/>
-      <c r="T1133" s="4"/>
-      <c r="V1133" s="4"/>
-      <c r="W1133" s="4"/>
-      <c r="X1133" s="4"/>
-      <c r="Y1133" s="4"/>
-      <c r="Z1133" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -30640,7 +30830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA33"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -30654,6 +30844,9 @@
         <v>12</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>13</v>
       </c>
     </row>
@@ -30661,10 +30854,10 @@
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
+      <c r="B3" s="2"/>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
       </c>
-      <c r="C3" s="2"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -30693,10 +30886,10 @@
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>14</v>
+      <c r="B4" s="2"/>
+      <c r="C4" s="5" t="s">
+        <v>70</v>
       </c>
-      <c r="C4" s="2"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -30725,10 +30918,10 @@
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>53</v>
+      <c r="B5" s="2"/>
+      <c r="C5" s="1" t="s">
+        <v>51</v>
       </c>
-      <c r="C5" s="2"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -30755,12 +30948,12 @@
     </row>
     <row r="6" spans="1:27" s="4" customFormat="1">
       <c r="A6" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>54</v>
+      <c r="B6" s="2"/>
+      <c r="C6" s="1" t="s">
+        <v>52</v>
       </c>
-      <c r="C6" s="2"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -30787,8 +30980,8 @@
     </row>
     <row r="7" spans="1:27" s="4" customFormat="1">
       <c r="A7" s="5"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -30815,12 +31008,12 @@
     </row>
     <row r="8" spans="1:27" s="4" customFormat="1">
       <c r="A8" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>56</v>
+      <c r="B8" s="2"/>
+      <c r="C8" s="1" t="s">
+        <v>54</v>
       </c>
-      <c r="C8" s="2"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -30847,8 +31040,8 @@
     </row>
     <row r="9" spans="1:27" s="4" customFormat="1">
       <c r="A9" s="5"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -30875,12 +31068,12 @@
     </row>
     <row r="10" spans="1:27" s="4" customFormat="1">
       <c r="A10" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>57</v>
+      <c r="B10" s="2"/>
+      <c r="C10" s="5" t="s">
+        <v>55</v>
       </c>
-      <c r="C10" s="2"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -30907,12 +31100,12 @@
     </row>
     <row r="11" spans="1:27" s="4" customFormat="1">
       <c r="A11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="2"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -30939,8 +31132,8 @@
     </row>
     <row r="12" spans="1:27" s="4" customFormat="1">
       <c r="A12" s="5"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -30967,12 +31160,14 @@
     </row>
     <row r="13" spans="1:27" s="4" customFormat="1">
       <c r="A13" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>20</v>
+      <c r="B13" s="2" t="s">
+        <v>71</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -30999,12 +31194,14 @@
     </row>
     <row r="14" spans="1:27" s="4" customFormat="1">
       <c r="A14" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>58</v>
+      <c r="B14" s="2" t="s">
+        <v>71</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -31031,8 +31228,8 @@
     </row>
     <row r="15" spans="1:27" s="4" customFormat="1">
       <c r="A15" s="5"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -31059,12 +31256,14 @@
     </row>
     <row r="16" spans="1:27" s="4" customFormat="1">
       <c r="A16" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>19</v>
+      <c r="B16" s="2" t="s">
+        <v>71</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -31093,8 +31292,8 @@
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -31121,12 +31320,14 @@
     </row>
     <row r="18" spans="1:27" s="4" customFormat="1">
       <c r="A18" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>26</v>
+      <c r="B18" s="2" t="s">
+        <v>71</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -31153,12 +31354,14 @@
     </row>
     <row r="19" spans="1:27" s="4" customFormat="1">
       <c r="A19" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>25</v>
+      <c r="B19" s="2" t="s">
+        <v>71</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -31185,12 +31388,14 @@
     </row>
     <row r="20" spans="1:27" s="4" customFormat="1">
       <c r="A20" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>21</v>
+      <c r="B20" s="2" t="s">
+        <v>71</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -31217,12 +31422,14 @@
     </row>
     <row r="21" spans="1:27" s="4" customFormat="1">
       <c r="A21" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>59</v>
+      <c r="B21" s="2" t="s">
+        <v>71</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -31251,8 +31458,8 @@
       <c r="A22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -31279,12 +31486,14 @@
     </row>
     <row r="23" spans="1:27" s="4" customFormat="1">
       <c r="A23" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>18</v>
+      <c r="B23" s="2" t="s">
+        <v>71</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -31311,8 +31520,8 @@
     </row>
     <row r="24" spans="1:27" s="4" customFormat="1">
       <c r="A24" s="5"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -31339,12 +31548,14 @@
     </row>
     <row r="25" spans="1:27" s="4" customFormat="1">
       <c r="A25" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>27</v>
+      <c r="B25" s="2" t="s">
+        <v>71</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -31373,10 +31584,10 @@
       <c r="A26" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>16</v>
+      <c r="B26" s="2"/>
+      <c r="C26" s="5" t="s">
+        <v>15</v>
       </c>
-      <c r="C26" s="2"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -31403,8 +31614,8 @@
     </row>
     <row r="27" spans="1:27" s="4" customFormat="1">
       <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="5"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -31431,12 +31642,12 @@
     </row>
     <row r="28" spans="1:27" s="4" customFormat="1">
       <c r="A28" s="5" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>24</v>
+      <c r="B28" s="2"/>
+      <c r="C28" s="1" t="s">
+        <v>23</v>
       </c>
-      <c r="C28" s="2"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -31463,7 +31674,7 @@
     </row>
     <row r="31" spans="1:27">
       <c r="A31" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:1">

</xml_diff>

<commit_message>
Merging selected changes from the release branch
The initial_catalyst_release branch got the updated checklist and
validator code, which needs to be brought back across to the master. The
various scripts and configs for running the site in production were also
updated and need to be merged into master.

Fixed a bug in the site CSS which was making the navbar the wrong size.

Added two new shell files for setting up the shell environment for
running the server during development (setup_dev_environment.sh) and
when running tests (setup_test_environment.sh).
</commit_message>
<xml_diff>
--- a/app/root/static/resources/validator/HICF_checklist/example_manifest.xlsx
+++ b/app/root/static/resources/validator/HICF_checklist/example_manifest.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28120" windowHeight="20160" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28120" windowHeight="20160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Manifest" sheetId="1" r:id="rId1"/>
+    <sheet name="example_manifest_with_unknowns." sheetId="1" r:id="rId1"/>
     <sheet name="Notes" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
   <si>
     <t>isolate</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Accession for the sample</t>
   </si>
   <si>
     <t>Accession for raw data i.e. fastq/bam files</t>
@@ -140,9 +137,6 @@
     <t>other classification</t>
   </si>
   <si>
-    <t>Example description</t>
-  </si>
-  <si>
     <t>Staphylococcus aureus 04-02981</t>
   </si>
   <si>
@@ -202,6 +196,48 @@
   </si>
   <si>
     <t>Describes the health care situation of a human host when the sample was obtained. Must be one of "inpatient" or "community". For non-human host, use "community".</t>
+  </si>
+  <si>
+    <t>ERS000001</t>
+  </si>
+  <si>
+    <t>not available: not collected</t>
+  </si>
+  <si>
+    <t>ERS000002</t>
+  </si>
+  <si>
+    <t>tetracyclin;S;40,erythromycin;R;ge50</t>
+  </si>
+  <si>
+    <t>ERS000003</t>
+  </si>
+  <si>
+    <t>Fully complete metadata</t>
+  </si>
+  <si>
+    <t>Partial metadata</t>
+  </si>
+  <si>
+    <t>Minimal metadata</t>
+  </si>
+  <si>
+    <t>uncultured bacterium</t>
+  </si>
+  <si>
+    <t>carriage</t>
+  </si>
+  <si>
+    <t>community</t>
+  </si>
+  <si>
+    <t>Accepts unknown</t>
+  </si>
+  <si>
+    <t>Accession for the sample, e.g. ERS000001</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
   <si>
     <t>antimicrobial resistance</t>
@@ -297,8 +333,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -377,7 +417,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -407,6 +447,8 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -436,6 +478,8 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -460,8 +504,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -471,7 +515,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="368300" y="6108700"/>
-          <a:ext cx="10452100" cy="7543800"/>
+          <a:ext cx="10452100" cy="10274300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -506,17 +550,16 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng" baseline="0"/>
             <a:t>Notes</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0" u="none"/>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="sng" baseline="0"/>
+            <a:rPr lang="en-US" sz="1100" b="0" u="sng" baseline="0"/>
             <a:t>Mandatory/optional</a:t>
           </a:r>
         </a:p>
@@ -526,19 +569,91 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t>Fields highlighted in </a:t>
+            <a:t>Fields highlighted in green are mandatory. Other fields are optional, subject to the dependencies specified below.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>green</a:t>
+            <a:rPr lang="en-US" sz="1100" b="0" u="sng" baseline="0"/>
+            <a:t>"Accepts unknown"</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t> are mandatory. Other fields are optional, subject to the dependencies specified below.</a:t>
+            <a:t>For some samples, such as historical samples of unknown provenance, it may be impossible to complete all mandatory fields. In such cases the value may be given as one of:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>"not available: not collected": not given because no value was collected</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>"not available: restricted access": not given because the data are restricted</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>"not available: to be reported later": not given but a value will be given at a later stage</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>"not applicable": not given because the checklist does not cover this eventuality</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>"obscured": deliberately not given</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>"temporarily obscured": not given but a value will be given at a later stage</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>These terms are accepted in any of the fields flagged as "Accepts unknown". The taxonomy and scientific name fields do not accept "unknown", but there are terms in the NCBI taxonomy tree to denote unknown species, e.g. ID 77133 represents "uncultured bacterium". Unknown organisms should be represented using similar valid terms from the taxonomy tree.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -580,15 +695,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t>If a sample is flagged as </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" u="none" baseline="0"/>
-            <a:t>not </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t>host associated, the four following fields are not required but "isolation source" becomes mandatory.</a:t>
+            <a:t>If a sample is flagged as not host associated, the four following fields are not required but "isolation source" becomes mandatory.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -606,7 +713,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t>When specifying the antimicrobial resistance for a sample, the field should contain a list of comma-separated values. Each value must contain three semi-colon separated fields: the name of the antibiotic, chosen from a curated list; susceptibility flag, either S (susceptible), I (intermediate), or R (resistant); the minimum inhibitory concentration (MIC) in microgrammes per millilitre (µg/ml). Optionally, a fourth, final field may be added, giving the name or location of the diagnostic centre that performed the resistance analysis.</a:t>
+            <a:t>When specifying the antimicrobial resistance for a sample, the field should contain a list of comma-separated values. Each value must contain three semi-colon separated fields: the name of the antibiotic, chosen from a curated list; susceptibility flag, either S (susceptible), I (intermediate), or R (resistant); the minimum inhibitory concentration (MIC) in microgrammes per millilitre (µg/ml). Optionally, a fourth, final field may be added, giving the name or location of the diagnostic centre that performed the resistance analysis. If the MIC value specifies a limit (e.g. &lt;=2), rather than an absolute value, it may be prefixed by one of: le (&lt;=), lt (&lt;), eq (=), gt (&gt;), ge (&gt;=).</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -615,7 +722,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
-            <a:t>Example: amoxicillin;S;2,piperacillin;S;4;WTSI;tetracycline;R;16;China</a:t>
+            <a:t>Example: amoxicillin;S;2,piperacillin;S;4;WTSI;tetracycline;R;16;China,vancomycin;R;ge32</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -742,6 +849,41 @@
             <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
             <a:t>BRENDA Tissue Ontology (BTO) in the EBI Ontology Browser: http://www.ebi.ac.uk/ontology-lookup/browse.do?ontName=BTO</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>EnvO</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>Environment Ontology: http://environmentontology.org/</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+            <a:t>EnvO in the EBI Ontology Browser: http://www.ebi.ac.uk/ontology-lookup/browse.do?ontName=ENVO</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1100" b="0" u="none" baseline="0"/>
@@ -1075,9 +1217,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1133"/>
+  <dimension ref="A1:Z1132"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1117,7 +1259,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>10</v>
@@ -1126,40 +1268,40 @@
         <v>11</v>
       </c>
       <c r="G1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="O1" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S1" s="5" t="s">
         <v>1</v>
@@ -1180,51 +1322,51 @@
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="13">
-        <v>1</v>
+      <c r="B2" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E2" s="4">
         <v>703339</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H2" s="4">
         <v>123</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="O2" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="P2" s="4"/>
       <c r="Q2" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R2" s="4"/>
       <c r="S2" s="4">
@@ -1232,7 +1374,7 @@
       </c>
       <c r="T2" s="4"/>
       <c r="U2" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
@@ -1241,24 +1383,63 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="5"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="4">
+        <v>703339</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
+      <c r="H3" s="4">
+        <v>123</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
+      <c r="Q3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="S3" s="4">
+        <v>630</v>
+      </c>
       <c r="T3" s="4"/>
+      <c r="U3" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
@@ -1266,21 +1447,54 @@
       <c r="Z3" s="4"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="C4" s="2"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="4">
+        <v>77133</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
+      <c r="I4" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
+      <c r="Q4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
       <c r="V4" s="4"/>
@@ -1482,6 +1696,8 @@
       <c r="Z12" s="4"/>
     </row>
     <row r="13" spans="1:26">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="2"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -30599,32 +30815,6 @@
       <c r="Y1132" s="4"/>
       <c r="Z1132" s="4"/>
     </row>
-    <row r="1133" spans="1:26">
-      <c r="A1133" s="4"/>
-      <c r="B1133" s="4"/>
-      <c r="C1133" s="2"/>
-      <c r="D1133" s="4"/>
-      <c r="E1133" s="4"/>
-      <c r="F1133" s="4"/>
-      <c r="G1133" s="4"/>
-      <c r="H1133" s="4"/>
-      <c r="J1133" s="4"/>
-      <c r="K1133" s="4"/>
-      <c r="L1133" s="4"/>
-      <c r="M1133" s="4"/>
-      <c r="N1133" s="4"/>
-      <c r="O1133" s="4"/>
-      <c r="P1133" s="4"/>
-      <c r="Q1133" s="4"/>
-      <c r="R1133" s="4"/>
-      <c r="S1133" s="4"/>
-      <c r="T1133" s="4"/>
-      <c r="V1133" s="4"/>
-      <c r="W1133" s="4"/>
-      <c r="X1133" s="4"/>
-      <c r="Y1133" s="4"/>
-      <c r="Z1133" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -30640,7 +30830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA33"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -30654,6 +30844,9 @@
         <v>12</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>13</v>
       </c>
     </row>
@@ -30661,10 +30854,10 @@
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
+      <c r="B3" s="2"/>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
       </c>
-      <c r="C3" s="2"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -30693,10 +30886,10 @@
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>14</v>
+      <c r="B4" s="2"/>
+      <c r="C4" s="5" t="s">
+        <v>70</v>
       </c>
-      <c r="C4" s="2"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -30725,10 +30918,10 @@
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>53</v>
+      <c r="B5" s="2"/>
+      <c r="C5" s="1" t="s">
+        <v>51</v>
       </c>
-      <c r="C5" s="2"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -30755,12 +30948,12 @@
     </row>
     <row r="6" spans="1:27" s="4" customFormat="1">
       <c r="A6" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>54</v>
+      <c r="B6" s="2"/>
+      <c r="C6" s="1" t="s">
+        <v>52</v>
       </c>
-      <c r="C6" s="2"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -30787,8 +30980,8 @@
     </row>
     <row r="7" spans="1:27" s="4" customFormat="1">
       <c r="A7" s="5"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -30815,12 +31008,12 @@
     </row>
     <row r="8" spans="1:27" s="4" customFormat="1">
       <c r="A8" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>56</v>
+      <c r="B8" s="2"/>
+      <c r="C8" s="1" t="s">
+        <v>54</v>
       </c>
-      <c r="C8" s="2"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -30847,8 +31040,8 @@
     </row>
     <row r="9" spans="1:27" s="4" customFormat="1">
       <c r="A9" s="5"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -30875,12 +31068,12 @@
     </row>
     <row r="10" spans="1:27" s="4" customFormat="1">
       <c r="A10" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>57</v>
+      <c r="B10" s="2"/>
+      <c r="C10" s="5" t="s">
+        <v>55</v>
       </c>
-      <c r="C10" s="2"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -30907,12 +31100,12 @@
     </row>
     <row r="11" spans="1:27" s="4" customFormat="1">
       <c r="A11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="2"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -30939,8 +31132,8 @@
     </row>
     <row r="12" spans="1:27" s="4" customFormat="1">
       <c r="A12" s="5"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -30967,12 +31160,14 @@
     </row>
     <row r="13" spans="1:27" s="4" customFormat="1">
       <c r="A13" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>20</v>
+      <c r="B13" s="2" t="s">
+        <v>71</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -30999,12 +31194,14 @@
     </row>
     <row r="14" spans="1:27" s="4" customFormat="1">
       <c r="A14" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>58</v>
+      <c r="B14" s="2" t="s">
+        <v>71</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -31031,8 +31228,8 @@
     </row>
     <row r="15" spans="1:27" s="4" customFormat="1">
       <c r="A15" s="5"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -31059,12 +31256,14 @@
     </row>
     <row r="16" spans="1:27" s="4" customFormat="1">
       <c r="A16" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>19</v>
+      <c r="B16" s="2" t="s">
+        <v>71</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -31093,8 +31292,8 @@
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -31121,12 +31320,14 @@
     </row>
     <row r="18" spans="1:27" s="4" customFormat="1">
       <c r="A18" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>26</v>
+      <c r="B18" s="2" t="s">
+        <v>71</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -31153,12 +31354,14 @@
     </row>
     <row r="19" spans="1:27" s="4" customFormat="1">
       <c r="A19" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>25</v>
+      <c r="B19" s="2" t="s">
+        <v>71</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -31185,12 +31388,14 @@
     </row>
     <row r="20" spans="1:27" s="4" customFormat="1">
       <c r="A20" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>21</v>
+      <c r="B20" s="2" t="s">
+        <v>71</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -31217,12 +31422,14 @@
     </row>
     <row r="21" spans="1:27" s="4" customFormat="1">
       <c r="A21" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>59</v>
+      <c r="B21" s="2" t="s">
+        <v>71</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -31251,8 +31458,8 @@
       <c r="A22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -31279,12 +31486,14 @@
     </row>
     <row r="23" spans="1:27" s="4" customFormat="1">
       <c r="A23" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>18</v>
+      <c r="B23" s="2" t="s">
+        <v>71</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -31311,8 +31520,8 @@
     </row>
     <row r="24" spans="1:27" s="4" customFormat="1">
       <c r="A24" s="5"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -31339,12 +31548,14 @@
     </row>
     <row r="25" spans="1:27" s="4" customFormat="1">
       <c r="A25" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>27</v>
+      <c r="B25" s="2" t="s">
+        <v>71</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -31373,10 +31584,10 @@
       <c r="A26" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>16</v>
+      <c r="B26" s="2"/>
+      <c r="C26" s="5" t="s">
+        <v>15</v>
       </c>
-      <c r="C26" s="2"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -31403,8 +31614,8 @@
     </row>
     <row r="27" spans="1:27" s="4" customFormat="1">
       <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="5"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -31431,12 +31642,12 @@
     </row>
     <row r="28" spans="1:27" s="4" customFormat="1">
       <c r="A28" s="5" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>24</v>
+      <c r="B28" s="2"/>
+      <c r="C28" s="1" t="s">
+        <v>23</v>
       </c>
-      <c r="C28" s="2"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -31463,7 +31674,7 @@
     </row>
     <row r="31" spans="1:27">
       <c r="A31" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:1">

</xml_diff>